<commit_message>
chi square bug fix
</commit_message>
<xml_diff>
--- a/2 - Language (Words)/Word Scaling Analysis Template.xlsx
+++ b/2 - Language (Words)/Word Scaling Analysis Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chand\OneDrive\Desktop\EMC-Scrotation-Station\2 - Language (Words)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emban\Documents\GitHub\EMC-Scrotation-Station\2 - Language (Words)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1426BBE2-1525-41D5-95BB-1C178D802B57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF1BB18-C9AA-44D4-B4DE-14BADDAC31DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3771" yWindow="3771" windowWidth="26332" windowHeight="13149" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -85,9 +85,6 @@
     <t>Xtick Locations</t>
   </si>
   <si>
-    <t>Char Scaling Analysis</t>
-  </si>
-  <si>
     <t>English Scaling</t>
   </si>
   <si>
@@ -107,6 +104,9 @@
   </si>
   <si>
     <t>Long English Scaling</t>
+  </si>
+  <si>
+    <t>Word Scaling Analysis</t>
   </si>
 </sst>
 </file>
@@ -473,22 +473,22 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="2" width="14.4609375" customWidth="1"/>
-    <col min="3" max="3" width="19.23046875" customWidth="1"/>
-    <col min="4" max="4" width="12.23046875" customWidth="1"/>
-    <col min="5" max="5" width="12.53515625" customWidth="1"/>
-    <col min="6" max="6" width="13.765625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.53515625" customWidth="1"/>
-    <col min="8" max="8" width="10.07421875" customWidth="1"/>
-    <col min="9" max="9" width="13.765625" customWidth="1"/>
-    <col min="10" max="10" width="12.765625" customWidth="1"/>
-    <col min="11" max="11" width="6.3046875" customWidth="1"/>
-    <col min="12" max="12" width="9.07421875" customWidth="1"/>
+    <col min="1" max="2" width="14.44140625" customWidth="1"/>
+    <col min="3" max="3" width="19.21875" customWidth="1"/>
+    <col min="4" max="4" width="12.21875" customWidth="1"/>
+    <col min="5" max="5" width="12.5546875" customWidth="1"/>
+    <col min="6" max="6" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" customWidth="1"/>
+    <col min="9" max="9" width="13.77734375" customWidth="1"/>
+    <col min="10" max="10" width="12.77734375" customWidth="1"/>
+    <col min="11" max="11" width="6.33203125" customWidth="1"/>
+    <col min="12" max="12" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -525,7 +525,7 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -540,16 +540,16 @@
         <v>17</v>
       </c>
       <c r="F2">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="H2">
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J2" t="s">
         <v>9</v>
@@ -569,7 +569,7 @@
         <v>2</v>
       </c>
       <c r="I3" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="J3" t="s">
         <v>9</v>
@@ -583,10 +583,10 @@
         <v>16</v>
       </c>
       <c r="G4" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="H4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I4" t="s">
         <v>25</v>
@@ -600,13 +600,13 @@
         <v>13</v>
       </c>
       <c r="G5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I5" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="J5" t="s">
         <v>9</v>

</xml_diff>